<commit_message>
Define 'kValue' and 'tau_sq' outside of main(); move auxiliary functions to file funcs.R (#1)
</commit_message>
<xml_diff>
--- a/n_values.xlsx
+++ b/n_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rritaz/Desktop/untitled folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sc/jobs/reviews/RSM/Repro-Man/RSM-01-2023-0003.R3/RVE-Meta-analysis-SMD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FA39C2-982A-CB42-8BAF-A7A50C72A823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B58C9A8-60CB-D74E-85DC-E18EF515F531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -359,7 +359,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -374,7 +374,35 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1000</v>
+      </c>
+    </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1000</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -382,6 +410,9 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1000</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -389,6 +420,9 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1000</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>

</xml_diff>